<commit_message>
Added if/else statement to switch gender text
</commit_message>
<xml_diff>
--- a/cover_letters.xlsx
+++ b/cover_letters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Company Name</t>
   </si>
@@ -34,28 +34,31 @@
     <t>Microsoft</t>
   </si>
   <si>
-    <t>David</t>
+    <t>Jane</t>
   </si>
   <si>
     <t>Peter</t>
   </si>
   <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Business Analyst Intern</t>
+  </si>
+  <si>
+    <t>2000 McGill College Ave, Montreal, QC H3A 3H3</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Blane</t>
+  </si>
+  <si>
     <t>Male</t>
-  </si>
-  <si>
-    <t>Business Analyst Intern</t>
-  </si>
-  <si>
-    <t>2000 McGill College Ave, Montreal, QC H3A 3H3</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>Blane</t>
   </si>
   <si>
     <t>Programmer Intern</t>
@@ -1357,13 +1360,13 @@
         <v>14</v>
       </c>
       <c r="D3" t="s" s="7">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="5"/>
     </row>

</xml_diff>